<commit_message>
Simplify language by using precedence rules
</commit_message>
<xml_diff>
--- a/local/scenarios/cough/Scenario.xlsx
+++ b/local/scenarios/cough/Scenario.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">ExampleProcess</t>
   </si>
   <si>
-    <t xml:space="preserve">DEFER()</t>
+    <t xml:space="preserve">DEFER();</t>
   </si>
 </sst>
 </file>
@@ -212,13 +212,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="76.14"/>
   </cols>
   <sheetData>

</xml_diff>